<commit_message>
finish sampletasklist review 100%
</commit_message>
<xml_diff>
--- a/SampleTaskList/Upload/MovieList.xlsx
+++ b/SampleTaskList/Upload/MovieList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>maleficent</t>
+  </si>
+  <si>
+    <t>toy story</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +424,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sample task list modifying
</commit_message>
<xml_diff>
--- a/SampleTaskList/Upload/MovieList.xlsx
+++ b/SampleTaskList/Upload/MovieList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>id</t>
   </si>
@@ -32,22 +32,13 @@
     <t>movie</t>
   </si>
   <si>
-    <t>Clash of Titans</t>
+    <t>daredevil</t>
   </si>
   <si>
-    <t>dune</t>
+    <t>superman</t>
   </si>
   <si>
-    <t>james bond</t>
-  </si>
-  <si>
-    <t>encanto</t>
-  </si>
-  <si>
-    <t>maleficent</t>
-  </si>
-  <si>
-    <t>toy story</t>
+    <t>justice league</t>
   </si>
 </sst>
 </file>
@@ -365,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,30 +399,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>